<commit_message>
Jig - Assembly, Magnetic Circuit, Stock Support, Main Body
Getting chain of referrals on dimensions to work well.  Realisation
that circuit needs bolting in to keep it at the right end of its nylon
hole.
</commit_message>
<xml_diff>
--- a/Assembly/Wheel Bill of Materials Cost Weight.xlsx
+++ b/Assembly/Wheel Bill of Materials Cost Weight.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37980" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-37360" yWindow="2000" windowWidth="37980" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Wheel BOM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Pack Price</t>
   </si>
@@ -81,9 +81,6 @@
     <t>12mm x 12mm x 12mm Pads, cut of 1mm</t>
   </si>
   <si>
-    <t>10mm x 3mm Side Pads &amp; Top Circuit, cuts of 3mm</t>
-  </si>
-  <si>
     <t>6mm rod x 100mm, cut of 1mm</t>
   </si>
   <si>
@@ -97,19 +94,35 @@
   </si>
   <si>
     <t>Packs to Order</t>
+  </si>
+  <si>
+    <t>10mm x 3mm Side Pads &amp; Top Circuit, cuts of 3mm.  Order qty is 1m</t>
+  </si>
+  <si>
+    <t>Metalbits Subtotal for one wheel, one car</t>
+  </si>
+  <si>
+    <t>Packs to Order per Car</t>
+  </si>
+  <si>
+    <t>Maplin Subtotal for one wheel, one car</t>
+  </si>
+  <si>
+    <t>This spreadsheet excludes shipping, as that decreases with volume a lot.  It includes VAT. Or should it?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0.0000_-;\-&quot;£&quot;* #,##0.0000_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-&quot;£&quot;* #,##0.00000_-;\-&quot;£&quot;* #,##0.00000_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +161,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,22 +192,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,12 +228,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,23 +577,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N15"/>
+  <dimension ref="B1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" style="4"/>
-    <col min="12" max="12" width="10.83203125" style="1"/>
-    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="4"/>
+    <col min="13" max="13" width="10.83203125" style="4"/>
+    <col min="15" max="15" width="10.83203125" style="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="9" customFormat="1" ht="30">
+    <row r="1" spans="2:17" s="9" customFormat="1" ht="45">
+      <c r="B1" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
@@ -551,87 +605,204 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:17">
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="F4">
-        <f>48*13</f>
-        <v>624</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="C4" s="1">
+        <f>3.32/2*1.2</f>
+        <v>1.9919999999999998</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2">
+        <f>C4/D4</f>
+        <v>1.9919999999999998</v>
+      </c>
+      <c r="G4">
+        <f>48*13*2</f>
+        <v>1248</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5">
+        <f>I4*F4</f>
+        <v>3.9839999999999995</v>
+      </c>
+      <c r="K4">
+        <f>4*G4</f>
+        <v>4992</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="5">
+        <f>5*F4</f>
+        <v>9.9599999999999991</v>
+      </c>
+      <c r="N4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5">
+    <row r="5" spans="2:17" ht="30">
+      <c r="B5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7">
+        <f>0.59*1.2</f>
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2">
+        <f>C5/D5</f>
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="G5">
         <f>48*(15+15+121)</f>
         <v>7248</v>
       </c>
-      <c r="G5" t="s">
-        <v>23</v>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5">
+        <f>I5*F5</f>
+        <v>5.6639999999999997</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K6" si="0">4*G5</f>
+        <v>28992</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="5">
+        <f>29*F5</f>
+        <v>20.532</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:17">
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <f>0.5*1.2</f>
+        <v>0.6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2">
+        <f>C6/D6</f>
+        <v>0.6</v>
+      </c>
+      <c r="G6">
         <f>48*101</f>
         <v>4848</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5">
+        <f>I6*F6</f>
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>19392</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="5">
+        <f>20*F6</f>
+        <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="7" spans="2:17" s="12" customFormat="1" ht="18">
+      <c r="B7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="J7" s="14">
+        <f>SUM(J4:J6)</f>
+        <v>12.648</v>
+      </c>
+      <c r="M7" s="14">
+        <f>SUM(M4:M6)</f>
+        <v>42.491999999999997</v>
+      </c>
+      <c r="O7" s="13"/>
+    </row>
+    <row r="11" spans="2:17">
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>15</v>
       </c>
-      <c r="N11" t="s">
+      <c r="Q11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:17">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -641,71 +812,94 @@
       <c r="D12">
         <v>6</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <f>C12/D12</f>
         <v>0.79</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>12</v>
       </c>
-      <c r="I12" s="5">
-        <f>F12*E12</f>
+      <c r="J12" s="5">
+        <f>G12*F12</f>
         <v>9.48</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" t="s">
+      <c r="M12" s="5"/>
+      <c r="N12" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="1">
+      <c r="O12" s="1">
         <v>7.99</v>
       </c>
-      <c r="M12" s="3">
+      <c r="P12" s="3">
         <v>42391</v>
       </c>
-      <c r="N12" t="s">
+      <c r="Q12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:17">
       <c r="B13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:17">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
         <v>7.72</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <f>425*100</f>
         <v>42500</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="8">
         <f>C15/D15</f>
         <v>1.8164705882352941E-4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="6">
         <f>PI()*8*300*48</f>
         <v>361911.47369354416</v>
       </c>
-      <c r="G15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="6">
-        <f>F15/D15</f>
-        <v>8.515564086906922</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="6">
+        <v>9</v>
+      </c>
+      <c r="J15" s="4">
+        <f>I15*C15</f>
+        <v>69.48</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="N15" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="3">
+      <c r="P15" s="3">
         <v>42391</v>
       </c>
-      <c r="N15" t="s">
+      <c r="Q15" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="16" spans="2:17" s="12" customFormat="1" ht="18">
+      <c r="B16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="J16" s="14">
+        <f>SUM(J13:J15)</f>
+        <v>69.48</v>
+      </c>
+      <c r="M16" s="14">
+        <f>SUM(M13:M15)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>